<commit_message>
library for v7 xamp
</commit_message>
<xml_diff>
--- a/export_abstract.xlsx
+++ b/export_abstract.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="0"/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
   <si>
     <t>Republic of the Philippines</t>
   </si>
@@ -29,19 +29,19 @@
     <t>ABSTRACT OF QUOTATIONS</t>
   </si>
   <si>
-    <t>For the quotation opened on March 11, 2020 at 19:01 pm</t>
+    <t>For the quotation opened on March 16, 2020 at 13:00 pm</t>
   </si>
   <si>
     <t>PR No.:</t>
   </si>
   <si>
-    <t>2020-03-0166</t>
+    <t>2020-02-00118</t>
   </si>
   <si>
     <t xml:space="preserve">PR Date: </t>
   </si>
   <si>
-    <t>March 25, 2020</t>
+    <t>February 26, 2020</t>
   </si>
   <si>
     <t>Mode of Procurement:</t>
@@ -53,25 +53,31 @@
     <t>RFQ No.:</t>
   </si>
   <si>
-    <t>2020-0095</t>
+    <t>2020-0085</t>
   </si>
   <si>
     <t xml:space="preserve">RFQ Date: </t>
   </si>
   <si>
+    <t>March 05, 2020</t>
+  </si>
+  <si>
     <t xml:space="preserve">Purpose: </t>
   </si>
   <si>
-    <t>asd</t>
+    <t>Support to Operation in the implementation of CMGP Programs for 1st Semester FY 2020</t>
   </si>
   <si>
     <t>ABC:</t>
   </si>
   <si>
+    <t>47,520</t>
+  </si>
+  <si>
     <t>Office:</t>
   </si>
   <si>
-    <t>FAD</t>
+    <t>LGMED</t>
   </si>
   <si>
     <t>ITEM DESCRIPTION</t>
@@ -86,13 +92,13 @@
     <t>ABC Per Item</t>
   </si>
   <si>
-    <t>Marinold Grill Co.</t>
-  </si>
-  <si>
-    <t>Power Electromechanical Data Support and Maintenance Co.</t>
-  </si>
-  <si>
-    <t>Paseo Premiere Hotel</t>
+    <t>Silicon Valley Computer Group Phil. Inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twis Trading </t>
+  </si>
+  <si>
+    <t>Panthertech Intl Marketing Corp.</t>
   </si>
   <si>
     <t>Quoted Price Per Item</t>
@@ -101,19 +107,44 @@
     <t>Total Price Per Item</t>
   </si>
   <si>
-    <t xml:space="preserve">3in1 Wireless Printer 
+    <t xml:space="preserve">Load card (globe 500)
 </t>
   </si>
   <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>14,700</t>
+    <t>piece</t>
+  </si>
+  <si>
+    <t>35,640</t>
+  </si>
+  <si>
+    <t>36,000</t>
+  </si>
+  <si>
+    <t>40,320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load card (smart 500)
+</t>
+  </si>
+  <si>
+    <t>11,880</t>
+  </si>
+  <si>
+    <t>12,000</t>
+  </si>
+  <si>
+    <t>13,440</t>
   </si>
   <si>
     <t>GRANDTOTAL</t>
   </si>
   <si>
+    <t>48,000</t>
+  </si>
+  <si>
+    <t>53,760</t>
+  </si>
+  <si>
     <t>Remarks:</t>
   </si>
   <si>
@@ -123,7 +154,7 @@
     <t>price(s), Which certify as fair and reasonable in the locality, as follows:</t>
   </si>
   <si>
-    <t>For Item(s) 1 to 1 to Marinold Grill Co.</t>
+    <t>For Item(s) 1 to 2 to Silicon Valley Computer Group Phil. Inc</t>
   </si>
   <si>
     <t>MAYBELLINE M. MONTEIRO</t>
@@ -233,15 +264,6 @@
     </font>
     <font>
       <b val="0"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
@@ -268,6 +290,15 @@
       <name val="Cambria"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b val="1"/>
       <i val="0"/>
       <strike val="0"/>
@@ -281,9 +312,9 @@
       <i val="1"/>
       <strike val="0"/>
       <u val="none"/>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Cambria"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b val="0"/>
@@ -461,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="77">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -495,18 +526,15 @@
     <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="5" numFmtId="49" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -525,10 +553,10 @@
     <xf xfId="0" fontId="5" numFmtId="164" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="8" numFmtId="164" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf xfId="0" fontId="7" numFmtId="164" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="8" numFmtId="164" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="7" numFmtId="164" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="164" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
@@ -567,7 +595,7 @@
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="9" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="8" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -630,47 +658,38 @@
     <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="9" numFmtId="0" fillId="2" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="9" numFmtId="0" fillId="2" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="9" numFmtId="164" fillId="2" borderId="13" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="13" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="13" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="2" borderId="13" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="9" numFmtId="164" fillId="5" borderId="13" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="9" numFmtId="164" fillId="5" borderId="13" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="10" numFmtId="0" fillId="2" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="10" numFmtId="0" fillId="2" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="10" numFmtId="0" fillId="2" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="10" numFmtId="164" fillId="2" borderId="13" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="10" numFmtId="164" fillId="5" borderId="13" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="10" numFmtId="164" fillId="5" borderId="13" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="9" numFmtId="164" fillId="2" borderId="13" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="13" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="13" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="13" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="164" fillId="2" borderId="13" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="164" fillId="5" borderId="13" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -678,62 +697,29 @@
     <xf xfId="0" fontId="11" numFmtId="164" fillId="5" borderId="13" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="10" numFmtId="164" fillId="2" borderId="13" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="10" numFmtId="164" fillId="2" borderId="13" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="10" numFmtId="164" fillId="2" borderId="13" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="1" numFmtId="164" fillId="6" borderId="13" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="10" numFmtId="164" fillId="2" borderId="13" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="10" numFmtId="164" fillId="2" borderId="13" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="164" fillId="6" borderId="13" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="10" numFmtId="164" fillId="2" borderId="13" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="12" numFmtId="49" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="12" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="8" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="8" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="3" numFmtId="164" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="8" numFmtId="164" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="7" numFmtId="164" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="8" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="13" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="13" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="13" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -1105,7 +1091,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" view="pageLayout" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="2.140625" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1146,106 +1132,106 @@
       </c>
     </row>
     <row r="8" spans="1:14" customHeight="1" ht="14.45">
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:14" customHeight="1" ht="24" s="1" customFormat="1">
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="47" t="s">
+      <c r="B10" s="44"/>
+      <c r="C10" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="47"/>
-      <c r="E10" s="43" t="s">
+      <c r="D10" s="46"/>
+      <c r="E10" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="45"/>
+      <c r="F10" s="44"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="40" t="s">
+      <c r="H10" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="42"/>
-      <c r="J10" s="43" t="s">
+      <c r="I10" s="41"/>
+      <c r="J10" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="44"/>
-      <c r="L10" s="40" t="s">
+      <c r="K10" s="43"/>
+      <c r="L10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="M10" s="41"/>
-      <c r="N10" s="42"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="41"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="47" t="s">
+      <c r="B11" s="44"/>
+      <c r="C11" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="47"/>
-      <c r="E11" s="43" t="s">
+      <c r="D11" s="46"/>
+      <c r="E11" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="45"/>
+      <c r="F11" s="44"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" s="42"/>
-      <c r="J11" s="36" t="s">
+      <c r="H11" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="37"/>
-      <c r="L11" s="48" t="s">
+      <c r="I11" s="41"/>
+      <c r="J11" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="M11" s="49"/>
-      <c r="N11" s="50"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" s="48"/>
+      <c r="N11" s="49"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="54">
-        <v>1</v>
-      </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="43" t="s">
+      <c r="A12" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="45"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="45"/>
+      <c r="E12" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="44"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="42"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="53"/>
+      <c r="H12" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="41"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="52"/>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="8"/>
@@ -1264,341 +1250,363 @@
       <c r="N13" s="8"/>
     </row>
     <row r="14" spans="1:14" customHeight="1" ht="28.5" s="1" customFormat="1">
-      <c r="A14" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="25" t="s">
+      <c r="A14" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="32" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="55" t="s">
+      <c r="G14" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24" t="s">
+      <c r="H14" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24" t="s">
+      <c r="I14" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="N14" s="24"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="23"/>
     </row>
     <row r="15" spans="1:14" customHeight="1" ht="27" s="1" customFormat="1">
-      <c r="A15" s="29"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="56" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="57" t="s">
-        <v>27</v>
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" s="54" t="s">
+        <v>29</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N15" s="10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:14" customHeight="1" ht="12" s="8" customFormat="1">
-      <c r="A16" s="60" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="61">
-        <v>1</v>
-      </c>
-      <c r="G16" s="62" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="63" t="s">
+      <c r="A16" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="64">
-        <v>1</v>
-      </c>
-      <c r="J16" s="65">
-        <v>1</v>
-      </c>
-      <c r="K16" s="72">
-        <v>2</v>
-      </c>
-      <c r="L16" s="73">
-        <v>2</v>
-      </c>
-      <c r="M16" s="76">
-        <v>5</v>
-      </c>
-      <c r="N16" s="77">
-        <v>5</v>
+      <c r="B16" s="55"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="57">
+        <v>72</v>
+      </c>
+      <c r="G16" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="58">
+        <v>500</v>
+      </c>
+      <c r="I16" s="62">
+        <v>495</v>
+      </c>
+      <c r="J16" s="63" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" s="65">
+        <v>500</v>
+      </c>
+      <c r="L16" s="65" t="s">
+        <v>33</v>
+      </c>
+      <c r="M16" s="65">
+        <v>560</v>
+      </c>
+      <c r="N16" s="65" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="66"/>
-      <c r="B17" s="67"/>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="70" t="s">
+      <c r="A17" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="57">
+        <v>24</v>
+      </c>
+      <c r="G17" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="J17" s="71">
-        <v>1</v>
-      </c>
-      <c r="K17" s="75" t="s">
-        <v>31</v>
-      </c>
-      <c r="L17" s="74">
-        <v>2</v>
-      </c>
-      <c r="M17" s="78" t="s">
-        <v>31</v>
-      </c>
-      <c r="N17" s="79">
-        <v>5</v>
+      <c r="H17" s="58">
+        <v>500</v>
+      </c>
+      <c r="I17" s="62">
+        <v>495</v>
+      </c>
+      <c r="J17" s="63" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" s="65">
+        <v>500</v>
+      </c>
+      <c r="L17" s="65" t="s">
+        <v>37</v>
+      </c>
+      <c r="M17" s="65">
+        <v>560</v>
+      </c>
+      <c r="N17" s="65" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="12"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
+      <c r="A18" s="64"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="66" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" s="67" t="s">
+        <v>18</v>
+      </c>
+      <c r="K18" s="68" t="s">
+        <v>39</v>
+      </c>
+      <c r="L18" s="65" t="s">
+        <v>40</v>
+      </c>
+      <c r="M18" s="68" t="s">
+        <v>39</v>
+      </c>
+      <c r="N18" s="65" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="19" spans="1:14" customHeight="1" ht="14.25" s="7" customFormat="1">
-      <c r="A19" s="80" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
+      <c r="A20" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
+      <c r="A21" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="14"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
+      <c r="A22" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
+      <c r="A24" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="23"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="14"/>
-      <c r="B26" s="81" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
       <c r="F26" s="9"/>
-      <c r="G26" s="83" t="s">
-        <v>37</v>
-      </c>
-      <c r="H26" s="20"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="85" t="s">
-        <v>38</v>
-      </c>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="14"/>
-      <c r="B27" s="82" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="84" t="s">
-        <v>39</v>
-      </c>
-      <c r="H27" s="18"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="86" t="s">
-        <v>40</v>
-      </c>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
+      <c r="G27" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="H27" s="17"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="74" t="s">
+        <v>48</v>
+      </c>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
       <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
+      <c r="G28" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="H28" s="17"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="75" t="s">
+        <v>50</v>
+      </c>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
     </row>
     <row r="30" spans="1:14">
-      <c r="A30" s="15"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
@@ -1617,12 +1625,8 @@
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
-      <c r="H31" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I31" s="88" t="s">
-        <v>42</v>
-      </c>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
@@ -1637,9 +1641,11 @@
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="87" t="s">
-        <v>43</v>
+      <c r="H32" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I32" s="73" t="s">
+        <v>52</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -1656,7 +1662,9 @@
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
+      <c r="I33" s="72" t="s">
+        <v>53</v>
+      </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
@@ -1664,9 +1672,7 @@
       <c r="N33" s="9"/>
     </row>
     <row r="34" spans="1:14">
-      <c r="A34" s="89" t="s">
-        <v>44</v>
-      </c>
+      <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -1682,8 +1688,8 @@
       <c r="N34" s="9"/>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="90" t="s">
-        <v>45</v>
+      <c r="A35" s="76" t="s">
+        <v>54</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -1700,8 +1706,8 @@
       <c r="N35" s="9"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36" s="91" t="s">
-        <v>46</v>
+      <c r="A36" s="76" t="s">
+        <v>55</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
@@ -1718,7 +1724,9 @@
       <c r="N36" s="9"/>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37" s="9"/>
+      <c r="A37" s="76" t="s">
+        <v>56</v>
+      </c>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
@@ -1794,15 +1802,16 @@
     <mergeCell ref="K14:L14"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="H14:H15"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A18:H18"/>
     <mergeCell ref="B27:E27"/>
-    <mergeCell ref="G26:K26"/>
+    <mergeCell ref="B28:E28"/>
     <mergeCell ref="G27:K27"/>
-    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="G28:K28"/>
     <mergeCell ref="L27:M27"/>
-    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="L28:M28"/>
     <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0" bottom="0" header="0.3" footer="0.3"/>

</xml_diff>